<commit_message>
Solution B12 is added
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/50c12d896f146c86/Desktop/crackerSheetSolutions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BC41BA8-8C95-4757-84E4-61CFD265FD79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{8BC41BA8-8C95-4757-84E4-61CFD265FD79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67E678CE-F526-4A20-8DE9-09AE062C7FC5}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1949,7 +1949,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="21">
@@ -1971,7 +1971,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="21">
@@ -2314,7 +2314,7 @@
         <v>43</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="21">
@@ -2440,7 +2440,7 @@
         <v>55</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Soution B45 is added
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/50c12d896f146c86/Desktop/crackerSheetSolutions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{8BC41BA8-8C95-4757-84E4-61CFD265FD79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67E678CE-F526-4A20-8DE9-09AE062C7FC5}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{8BC41BA8-8C95-4757-84E4-61CFD265FD79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4605A041-A6FF-4B6B-9C8C-8A6DCD50EEF2}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="B44" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2325,7 +2325,7 @@
         <v>44</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="21">

</xml_diff>

<commit_message>
We have added solution B10
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/50c12d896f146c86/Desktop/crackerSheetSolutions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{8BC41BA8-8C95-4757-84E4-61CFD265FD79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4605A041-A6FF-4B6B-9C8C-8A6DCD50EEF2}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{8BC41BA8-8C95-4757-84E4-61CFD265FD79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{659AEF32-C234-4A06-9EDA-95E98DEE4997}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B44" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1916,7 +1916,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Solution B11 and Solution B57 are added
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/50c12d896f146c86/Desktop/crackerSheetSolutions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{8BC41BA8-8C95-4757-84E4-61CFD265FD79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{659AEF32-C234-4A06-9EDA-95E98DEE4997}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{8BC41BA8-8C95-4757-84E4-61CFD265FD79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05513B26-C47C-497E-B52C-47CE29CF020F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1960,7 +1960,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Changes to the CrackerSheet
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/50c12d896f146c86/Desktop/crackerSheetSolutions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{8BC41BA8-8C95-4757-84E4-61CFD265FD79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05513B26-C47C-497E-B52C-47CE29CF020F}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{8BC41BA8-8C95-4757-84E4-61CFD265FD79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44965293-6EFA-45CA-B44E-E2AB0E09F556}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:C11"/>
+    <sheetView tabSelected="1" topLeftCell="B56" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2347,7 +2347,7 @@
         <v>46</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Added Solution B297, it is the implementation of queue using an array
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/50c12d896f146c86/Desktop/crackerSheetSolutions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{8BC41BA8-8C95-4757-84E4-61CFD265FD79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44965293-6EFA-45CA-B44E-E2AB0E09F556}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{8BC41BA8-8C95-4757-84E4-61CFD265FD79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B4E2717-E6DD-4A1D-BADC-17FFC22E6C19}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B56" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="B293" workbookViewId="0">
+      <selection activeCell="C297" sqref="C297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -4962,7 +4962,7 @@
         <v>286</v>
       </c>
       <c r="C296" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="297" spans="1:3" ht="21">
@@ -4973,7 +4973,7 @@
         <v>287</v>
       </c>
       <c r="C297" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="298" spans="1:3" ht="21">

</xml_diff>